<commit_message>
added Jessie's 'Spray Mite Survey' data as 'ipm _trial_2021.xlsx', updating code
</commit_message>
<xml_diff>
--- a/data/rrv_mite_survey_master.xlsx
+++ b/data/rrv_mite_survey_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/DISSERTATION/MANUSCRIPT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="114_{A1ACD467-6F52-452F-8CA7-A698329C7C41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B5833CB2-9AFA-42CC-B7B7-EC1B46AEFEF7}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="114_{A1ACD467-6F52-452F-8CA7-A698329C7C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4117EF3-581F-443B-B6B1-FCB86C51E82A}"/>
   <bookViews>
-    <workbookView xWindow="-6930" yWindow="4140" windowWidth="16290" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="3000" windowWidth="9975" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mite_survey_master" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3774" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3774" uniqueCount="468">
   <si>
     <t>sample_no</t>
   </si>
@@ -1428,18 +1428,6 @@
   </si>
   <si>
     <t>Santa Rosa</t>
-  </si>
-  <si>
-    <t>RRV Pheno 12</t>
-  </si>
-  <si>
-    <t>RRV Pheno 11</t>
-  </si>
-  <si>
-    <t>RRV Pheno 14</t>
-  </si>
-  <si>
-    <t>RRV Pheno 13</t>
   </si>
   <si>
     <t>lon_lat</t>
@@ -2339,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S486"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A437" workbookViewId="0">
-      <selection activeCell="E467" sqref="E467"/>
+    <sheetView tabSelected="1" topLeftCell="A464" workbookViewId="0">
+      <selection activeCell="C371" sqref="C371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -2408,7 +2396,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>341</v>
@@ -18923,7 +18911,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>466</v>
+        <v>431</v>
       </c>
       <c r="C369" s="5">
         <v>43991</v>
@@ -18974,7 +18962,7 @@
         <v>369</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>465</v>
+        <v>432</v>
       </c>
       <c r="C370" s="5">
         <v>43991</v>
@@ -19025,7 +19013,7 @@
         <v>370</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>468</v>
+        <v>433</v>
       </c>
       <c r="C371" s="5">
         <v>43991</v>
@@ -19076,7 +19064,7 @@
         <v>371</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>467</v>
+        <v>434</v>
       </c>
       <c r="C372" s="5">
         <v>43991</v>
@@ -24788,7 +24776,7 @@
         <v>483</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C484" s="5">
         <v>44273</v>
@@ -25168,18 +25156,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25203,14 +25191,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18214261-A5B8-46A6-8EA9-D141AF47C781}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3B13BC9-D801-4C64-8AB5-CC109F2868F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -25218,4 +25198,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18214261-A5B8-46A6-8EA9-D141AF47C781}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>